<commit_message>
Signed-off-by: michel michael <m.michel@onlineformapro.com> Modif ajout de la classe PhpSpreadSheet pour import et export en xlsx
ATTENTION: 	MODIFIER LE FORMAT DE DATE
AJOUTER LA CREATION DE COMPETITION ETC...
</commit_message>
<xml_diff>
--- a/Datas/ski.xlsx
+++ b/Datas/ski.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\ApiSki\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{C9D19578-2A2E-4C11-8D4D-55A8F645063F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{6D90DC83-5348-42F4-BEDE-37E10676AD18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2670" yWindow="360" windowWidth="15375" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compétition Ski" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>station</t>
   </si>
@@ -50,75 +50,18 @@
     <t>temps_epreuve</t>
   </si>
   <si>
-    <t>Les 2 Alpes</t>
-  </si>
-  <si>
-    <t>MICHEL</t>
-  </si>
-  <si>
-    <t>Michael</t>
-  </si>
-  <si>
-    <t>micpiwo@hotmail,fr</t>
-  </si>
-  <si>
-    <t>https://picsum.photos/200/300</t>
-  </si>
-  <si>
-    <t>M2</t>
-  </si>
-  <si>
-    <t>Les 7 Laux</t>
-  </si>
-  <si>
-    <t>BOB</t>
-  </si>
-  <si>
-    <t>EPONGE</t>
-  </si>
-  <si>
-    <t>bob@hotmai.fr</t>
-  </si>
-  <si>
-    <t>SNOWBOARD</t>
-  </si>
-  <si>
-    <t>TEST 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GLISSE </t>
-  </si>
-  <si>
-    <t>Sophie</t>
-  </si>
-  <si>
-    <t>sophie@cool,fr</t>
-  </si>
-  <si>
-    <t>M4</t>
+    <t>a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,22 +81,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,23 +391,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -509,99 +437,61 @@
         <v>9</v>
       </c>
       <c r="B2" s="1">
-        <v>44208</v>
+        <v>44545</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1">
-        <v>31043</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2">
-        <v>1.2565200000000001</v>
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="5">
-        <v>44326</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>17</v>
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44208</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
       </c>
       <c r="E3" s="1">
-        <v>28775</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>19</v>
+        <v>31043</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
       </c>
       <c r="I3">
-        <v>2.214585</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5">
-        <v>44206</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1">
-        <v>36934</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4">
-        <v>1.211425</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{83FF8F3A-E03D-44BA-9F90-16FC156AFC04}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{95263263-8796-4669-A3F8-011C8A29548B}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{35F56D2E-A134-4E1D-88F0-734D5E674373}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{20D6996C-9804-40E5-B7CB-270F09266A93}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{2E852432-3309-4F43-A915-A289473D5C77}"/>
-    <hyperlink ref="G4" r:id="rId6" xr:uid="{EAF027D9-DCCA-411E-8871-AE50778487CD}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>